<commit_message>
Sai 150 changes commit
</commit_message>
<xml_diff>
--- a/Use Tax_Disptacher/Data/Config.xlsx
+++ b/Use Tax_Disptacher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Tax-Use-Automation\Use Tax_Disptacher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE06C2B-DC7A-49F5-8623-B3E66EB68E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9FFB3F-6780-45A7-A1E2-9ECEA3A64849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t>ERP</t>
   </si>
   <si>
-    <t>Use Tax</t>
-  </si>
-  <si>
     <t>Use Tax_Dispatcher</t>
   </si>
   <si>
@@ -340,7 +337,10 @@
     <t>Invoice FolderPath</t>
   </si>
   <si>
-    <t>UAT</t>
+    <t>UseTax</t>
+  </si>
+  <si>
+    <t>Dev</t>
   </si>
 </sst>
 </file>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -818,7 +818,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -841,7 +841,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>19</v>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z983"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2007,18 +2007,18 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
         <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -2095,124 +2095,124 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
         <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
         <v>74</v>
-      </c>
-      <c r="B32" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
         <v>76</v>
-      </c>
-      <c r="B33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
         <v>78</v>
-      </c>
-      <c r="B34" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
         <v>80</v>
-      </c>
-      <c r="B35" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
         <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
         <v>94</v>
-      </c>
-      <c r="B38" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="str">
         <f ca="1">_xlfn.CONCAT("\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\",TEXT(TODAY(),"yyyy"),"\000FY",TEXT(TODAY(),"yy")," AZ FL PA TX Use Tax Reports\")</f>
-        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\2024\000FY24 AZ FL PA TX Use Tax Reports\</v>
+        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\2025\000FY25 AZ FL PA TX Use Tax Reports\</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30.65" customHeight="1">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B43" s="3" t="str">
         <f ca="1">_xlfn.CONCAT("\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\AZ-FL-PA-TX Invoices to verify (Monthly)","\",TEXT(TODAY(),"yyyy"),"\",TEXT(EOMONTH(TODAY(),-1),"mmmm"))</f>
-        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\AZ-FL-PA-TX Invoices to verify (Monthly)\2024\September</v>
+        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\AZ-FL-PA-TX Invoices to verify (Monthly)\2025\December</v>
       </c>
       <c r="C43" s="11"/>
     </row>
@@ -3167,7 +3167,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3227,7 +3227,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3243,7 +3243,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3259,37 +3259,37 @@
         <v>55</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
previous month date time issue resolved and published
</commit_message>
<xml_diff>
--- a/Use Tax_Disptacher/Data/Config.xlsx
+++ b/Use Tax_Disptacher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Tax-Use-Automation\Use Tax_Disptacher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Tax-Use-Automation\Use Tax_Disptacher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9FFB3F-6780-45A7-A1E2-9ECEA3A64849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A3B765-17AC-466A-9F5B-5875BD6A2A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -340,7 +340,7 @@
     <t>UseTax</t>
   </si>
   <si>
-    <t>Dev</t>
+    <t>Prod</t>
   </si>
 </sst>
 </file>
@@ -768,15 +768,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -836,7 +836,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1853,16 +1853,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="65.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1899,7 +1899,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1994,7 +1994,7 @@
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2203,16 +2203,16 @@
       </c>
       <c r="B42" t="str">
         <f ca="1">_xlfn.CONCAT("\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\",TEXT(TODAY(),"yyyy"),"\000FY",TEXT(TODAY(),"yy")," AZ FL PA TX Use Tax Reports\")</f>
-        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\2025\000FY25 AZ FL PA TX Use Tax Reports\</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30.65" customHeight="1">
+        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\2026\000FY26 AZ FL PA TX Use Tax Reports\</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30.6" customHeight="1">
       <c r="A43" t="s">
         <v>98</v>
       </c>
       <c r="B43" s="3" t="str">
         <f ca="1">_xlfn.CONCAT("\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\AZ-FL-PA-TX Invoices to verify (Monthly)","\",TEXT(TODAY(),"yyyy"),"\",TEXT(EOMONTH(TODAY(),-1),"mmmm"))</f>
-        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\AZ-FL-PA-TX Invoices to verify (Monthly)\2025\December</v>
+        <v>\\twcfileshp01\usershares$\Accounting\Sales Tax\Use Tax\AZ-FL-PA-TX Invoices to verify (Monthly)\2026\December</v>
       </c>
       <c r="C43" s="11"/>
     </row>
@@ -3166,16 +3166,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3221,6 +3221,9 @@
       <c r="B2" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="7" t="s">
@@ -3229,6 +3232,9 @@
       <c r="B3" s="10" t="s">
         <v>89</v>
       </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="7" t="s">
@@ -3237,6 +3243,9 @@
       <c r="B4" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="7" t="s">
@@ -3245,6 +3254,9 @@
       <c r="B5" s="10" t="s">
         <v>90</v>
       </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -3253,6 +3265,9 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="7" t="s">
@@ -3261,6 +3276,9 @@
       <c r="B7" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -3269,6 +3287,9 @@
       <c r="B8" s="7" t="s">
         <v>59</v>
       </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
       <c r="D8" s="7" t="s">
         <v>96</v>
       </c>
@@ -3280,6 +3301,9 @@
       <c r="B9" t="s">
         <v>62</v>
       </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
       <c r="D9" t="s">
         <v>97</v>
       </c>
@@ -3290,6 +3314,9 @@
       </c>
       <c r="B10" s="9" t="s">
         <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>